<commit_message>
TEST CASE 374 e colonne F, G, H, I, L, M, O, P
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_AMBWEB/20.15.00/accreditamento-checklist_V8.1.3.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_AMBWEB/20.15.00/accreditamento-checklist_V8.1.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lavoro\2023_BTU\Modello_Standard_CDA\AMB\Accreditamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85B2E87-4F95-4128-A341-466B42E7A493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53E8F31-35D7-4382-89CA-B9FE474ED43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2271" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="957">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4765,6 +4765,39 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.180.4.4.3517dda38fa520834444f1572c6764ee49550efac86304de47a2f591f91ded30.e3a6c3b88f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-23T17:30:15Z</t>
+  </si>
+  <si>
+    <t>a7023c78a737df45</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.180.4.4.5949a919a8471dd8455aeb88dd57262f47b8c03771f66723b180437630f24060.d540359bf7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di token, ma il flusso applicativo prosegue con la produzione del referto. La correzione può essere fatta da un utente amministratore, tramite front-end</t>
+  </si>
+  <si>
+    <t>Viene segnalato un errore di timeout, ma il flusso applicativo prosegue con la produzione del referto. La correzione può essere fatta da un utente amministratore, tramite front-end</t>
+  </si>
+  <si>
+    <t>Viene segnalato l'errore ritornato dal Gateway. La correzione può essere fatta da un utente amministratore, tramite front-end, attivando l'obbligatorietà del campo</t>
+  </si>
+  <si>
+    <t>Viene segnalato l'errore ritornato dal Gateway. La correzione può essere fatta dall'utente stesso, modificando il codice fiscale sul front-end</t>
+  </si>
+  <si>
+    <t>Viene segnalato l'errore ritornato dal Gateway. La correzione può essere fatta da un utente amministratore, tramite front-end, corregendo il template di generazione del CDA</t>
+  </si>
+  <si>
+    <t>Viene segnalato l'errore ritornato dal Gateway. La correzione può essere fatta dall'utente stesso, completandoi dati del paziente i dati del paziente</t>
+  </si>
+  <si>
+    <t>Viene segnalato l'errore ritornato dal Gateway. La modifica alla configurazione amministratore, tramite front-end</t>
+  </si>
+  <si>
+    <t>Viene segnalato l'errore ritornato dal Gateway. L'utente può completare i dati tramite frontend e rilanciare la validazione</t>
   </si>
 </sst>
 </file>
@@ -7661,10 +7694,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B156" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="K39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P157" sqref="P157"/>
+      <selection pane="bottomRight" activeCell="P169" sqref="P169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8948,9 +8981,11 @@
       <c r="N39" s="25" t="s">
         <v>918</v>
       </c>
-      <c r="O39" s="25"/>
+      <c r="O39" s="25" t="s">
+        <v>845</v>
+      </c>
       <c r="P39" s="25" t="s">
-        <v>912</v>
+        <v>949</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26" t="s">
@@ -9240,9 +9275,11 @@
       <c r="N47" s="25" t="s">
         <v>918</v>
       </c>
-      <c r="O47" s="25"/>
+      <c r="O47" s="25" t="s">
+        <v>845</v>
+      </c>
       <c r="P47" s="25" t="s">
-        <v>912</v>
+        <v>950</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26" t="s">
@@ -13108,8 +13145,12 @@
       <c r="N158" s="25" t="s">
         <v>924</v>
       </c>
-      <c r="O158" s="25"/>
-      <c r="P158" s="25"/>
+      <c r="O158" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P158" s="25" t="s">
+        <v>951</v>
+      </c>
       <c r="Q158" s="25"/>
       <c r="R158" s="26" t="s">
         <v>136</v>
@@ -13160,8 +13201,12 @@
       <c r="N159" s="25" t="s">
         <v>925</v>
       </c>
-      <c r="O159" s="25"/>
-      <c r="P159" s="25"/>
+      <c r="O159" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P159" s="25" t="s">
+        <v>952</v>
+      </c>
       <c r="Q159" s="25"/>
       <c r="R159" s="26" t="s">
         <v>136</v>
@@ -13212,8 +13257,12 @@
       <c r="N160" s="25" t="s">
         <v>926</v>
       </c>
-      <c r="O160" s="25"/>
-      <c r="P160" s="25"/>
+      <c r="O160" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P160" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q160" s="25"/>
       <c r="R160" s="26" t="s">
         <v>136</v>
@@ -13264,8 +13313,12 @@
       <c r="N161" s="25" t="s">
         <v>927</v>
       </c>
-      <c r="O161" s="25"/>
-      <c r="P161" s="25"/>
+      <c r="O161" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P161" s="25" t="s">
+        <v>954</v>
+      </c>
       <c r="Q161" s="25"/>
       <c r="R161" s="26" t="s">
         <v>136</v>
@@ -13316,8 +13369,12 @@
       <c r="N162" s="25" t="s">
         <v>928</v>
       </c>
-      <c r="O162" s="25"/>
-      <c r="P162" s="25"/>
+      <c r="O162" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P162" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q162" s="25"/>
       <c r="R162" s="26" t="s">
         <v>136</v>
@@ -13368,8 +13425,12 @@
       <c r="N163" s="25" t="s">
         <v>929</v>
       </c>
-      <c r="O163" s="25"/>
-      <c r="P163" s="25"/>
+      <c r="O163" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P163" s="25" t="s">
+        <v>955</v>
+      </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26" t="s">
         <v>136</v>
@@ -13420,8 +13481,12 @@
       <c r="N164" s="25" t="s">
         <v>930</v>
       </c>
-      <c r="O164" s="25"/>
-      <c r="P164" s="25"/>
+      <c r="O164" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P164" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q164" s="25"/>
       <c r="R164" s="26" t="s">
         <v>136</v>
@@ -13472,8 +13537,12 @@
       <c r="N165" s="25" t="s">
         <v>931</v>
       </c>
-      <c r="O165" s="25"/>
-      <c r="P165" s="25"/>
+      <c r="O165" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P165" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q165" s="25"/>
       <c r="R165" s="26" t="s">
         <v>136</v>
@@ -13524,8 +13593,12 @@
       <c r="N166" s="25" t="s">
         <v>932</v>
       </c>
-      <c r="O166" s="25"/>
-      <c r="P166" s="25"/>
+      <c r="O166" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P166" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q166" s="25"/>
       <c r="R166" s="26" t="s">
         <v>136</v>
@@ -13576,8 +13649,12 @@
       <c r="N167" s="25" t="s">
         <v>933</v>
       </c>
-      <c r="O167" s="25"/>
-      <c r="P167" s="25"/>
+      <c r="O167" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P167" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26" t="s">
         <v>136</v>
@@ -13628,8 +13705,12 @@
       <c r="N168" s="25" t="s">
         <v>934</v>
       </c>
-      <c r="O168" s="25"/>
-      <c r="P168" s="25"/>
+      <c r="O168" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P168" s="25" t="s">
+        <v>956</v>
+      </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26" t="s">
         <v>136</v>
@@ -13680,8 +13761,12 @@
       <c r="N169" t="s">
         <v>942</v>
       </c>
-      <c r="O169" s="25"/>
-      <c r="P169" s="25"/>
+      <c r="O169" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P169" s="25" t="s">
+        <v>956</v>
+      </c>
       <c r="Q169" s="25"/>
       <c r="R169" s="26" t="s">
         <v>136</v>
@@ -13732,8 +13817,12 @@
       <c r="N170" s="25" t="s">
         <v>935</v>
       </c>
-      <c r="O170" s="25"/>
-      <c r="P170" s="25"/>
+      <c r="O170" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P170" s="25" t="s">
+        <v>956</v>
+      </c>
       <c r="Q170" s="25"/>
       <c r="R170" s="26" t="s">
         <v>136</v>
@@ -13784,8 +13873,12 @@
       <c r="N171" s="25" t="s">
         <v>936</v>
       </c>
-      <c r="O171" s="25"/>
-      <c r="P171" s="25"/>
+      <c r="O171" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P171" s="25" t="s">
+        <v>956</v>
+      </c>
       <c r="Q171" s="25"/>
       <c r="R171" s="26" t="s">
         <v>136</v>
@@ -13836,8 +13929,12 @@
       <c r="N172" s="25" t="s">
         <v>937</v>
       </c>
-      <c r="O172" s="25"/>
-      <c r="P172" s="25"/>
+      <c r="O172" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P172" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q172" s="25"/>
       <c r="R172" s="26" t="s">
         <v>136</v>
@@ -13888,8 +13985,12 @@
       <c r="N173" s="25" t="s">
         <v>938</v>
       </c>
-      <c r="O173" s="25"/>
-      <c r="P173" s="25"/>
+      <c r="O173" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P173" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q173" s="25"/>
       <c r="R173" s="26" t="s">
         <v>136</v>
@@ -13940,8 +14041,12 @@
       <c r="N174" s="25" t="s">
         <v>939</v>
       </c>
-      <c r="O174" s="25"/>
-      <c r="P174" s="25"/>
+      <c r="O174" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P174" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q174" s="25"/>
       <c r="R174" s="26" t="s">
         <v>136</v>
@@ -13992,8 +14097,12 @@
       <c r="N175" s="25" t="s">
         <v>940</v>
       </c>
-      <c r="O175" s="25"/>
-      <c r="P175" s="25"/>
+      <c r="O175" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P175" s="25" t="s">
+        <v>955</v>
+      </c>
       <c r="Q175" s="25"/>
       <c r="R175" s="26" t="s">
         <v>136</v>
@@ -14044,8 +14153,12 @@
       <c r="N176" s="25" t="s">
         <v>941</v>
       </c>
-      <c r="O176" s="25"/>
-      <c r="P176" s="25"/>
+      <c r="O176" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="P176" s="25" t="s">
+        <v>953</v>
+      </c>
       <c r="Q176" s="25"/>
       <c r="R176" s="26" t="s">
         <v>136</v>
@@ -18067,7 +18180,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="264" customHeight="1" thickBot="1">
+    <row r="295" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A295" s="20">
         <v>288</v>
       </c>
@@ -18101,7 +18214,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
+    <row r="296" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A296" s="20">
         <v>289</v>
       </c>
@@ -18135,7 +18248,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="14.25" customHeight="1">
+    <row r="297" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A297" s="20">
         <v>290</v>
       </c>
@@ -18169,7 +18282,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="14.25" customHeight="1">
+    <row r="298" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A298" s="20">
         <v>291</v>
       </c>
@@ -18203,7 +18316,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="14.25" customHeight="1">
+    <row r="299" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A299" s="20">
         <v>292</v>
       </c>
@@ -18237,7 +18350,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="14.25" customHeight="1">
+    <row r="300" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A300" s="20">
         <v>293</v>
       </c>
@@ -18271,7 +18384,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="14.25" customHeight="1">
+    <row r="301" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A301" s="20">
         <v>294</v>
       </c>
@@ -18305,7 +18418,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="14.25" customHeight="1">
+    <row r="302" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A302" s="20">
         <v>295</v>
       </c>
@@ -18339,7 +18452,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="14.25" customHeight="1">
+    <row r="303" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A303" s="20">
         <v>296</v>
       </c>
@@ -18373,7 +18486,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="14.25" customHeight="1">
+    <row r="304" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A304" s="20">
         <v>297</v>
       </c>
@@ -18407,7 +18520,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="14.25" customHeight="1">
+    <row r="305" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A305" s="20">
         <v>298</v>
       </c>
@@ -18441,7 +18554,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="14.25" customHeight="1">
+    <row r="306" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A306" s="20">
         <v>299</v>
       </c>
@@ -18475,7 +18588,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="14.25" customHeight="1">
+    <row r="307" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A307" s="20">
         <v>300</v>
       </c>
@@ -18509,7 +18622,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="14.25" customHeight="1">
+    <row r="308" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A308" s="20">
         <v>301</v>
       </c>
@@ -18543,7 +18656,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="14.25" customHeight="1">
+    <row r="309" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A309" s="20">
         <v>302</v>
       </c>
@@ -18577,7 +18690,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
+    <row r="310" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A310" s="20">
         <v>303</v>
       </c>
@@ -19971,7 +20084,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="242.25" customHeight="1" thickBot="1">
+    <row r="351" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A351" s="20">
         <v>344</v>
       </c>
@@ -20005,7 +20118,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="242.25" customHeight="1" thickBot="1">
+    <row r="352" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A352" s="20">
         <v>345</v>
       </c>
@@ -20039,7 +20152,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="315" customHeight="1">
+    <row r="353" spans="1:20" ht="9.9499999999999993" customHeight="1">
       <c r="A353" s="20">
         <v>346</v>
       </c>
@@ -20073,7 +20186,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="259.5" customHeight="1" thickBot="1">
+    <row r="354" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A354" s="20">
         <v>347</v>
       </c>
@@ -20651,7 +20764,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="249.75" customHeight="1" thickBot="1">
+    <row r="371" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A371" s="20">
         <v>364</v>
       </c>
@@ -20685,7 +20798,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="249.75" customHeight="1" thickBot="1">
+    <row r="372" spans="1:20" ht="9.9499999999999993" customHeight="1" thickBot="1">
       <c r="A372" s="20">
         <v>365</v>
       </c>
@@ -20991,7 +21104,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="14.25" customHeight="1">
+    <row r="381" spans="1:20" ht="21" customHeight="1">
       <c r="A381" s="20">
         <v>374</v>
       </c>
@@ -21007,11 +21120,21 @@
       <c r="E381" s="22" t="s">
         <v>787</v>
       </c>
-      <c r="F381" s="23"/>
-      <c r="G381" s="24"/>
-      <c r="H381" s="24"/>
-      <c r="I381" s="24"/>
-      <c r="J381" s="25"/>
+      <c r="F381" s="23">
+        <v>45253</v>
+      </c>
+      <c r="G381" s="24" t="s">
+        <v>946</v>
+      </c>
+      <c r="H381" s="24" t="s">
+        <v>947</v>
+      </c>
+      <c r="I381" s="24" t="s">
+        <v>948</v>
+      </c>
+      <c r="J381" s="25" t="s">
+        <v>136</v>
+      </c>
       <c r="K381" s="25"/>
       <c r="L381" s="25"/>
       <c r="M381" s="25"/>
@@ -21019,7 +21142,9 @@
       <c r="O381" s="25"/>
       <c r="P381" s="25"/>
       <c r="Q381" s="25"/>
-      <c r="R381" s="26"/>
+      <c r="R381" s="26" t="s">
+        <v>136</v>
+      </c>
       <c r="S381" s="27"/>
       <c r="T381" s="28" t="s">
         <v>47</v>
@@ -21059,7 +21184,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="14.25" hidden="1" customHeight="1">
+    <row r="383" spans="1:20" ht="1.5" hidden="1" customHeight="1">
       <c r="A383" s="20">
         <v>376</v>
       </c>

</xml_diff>

<commit_message>
update checklist CT 40
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_AMBWEB/20.15.00/accreditamento-checklist_V8.1.3.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/AREAS_AMBWEB/20.15.00/accreditamento-checklist_V8.1.3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lavoro\2023_BTU\Modello_Standard_CDA\AMB\Accreditamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B2EDCC-235E-4B40-A21B-292B6F846DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E8B327-CE5E-4C04-B7E9-6C55AE1A0412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4752,9 +4752,6 @@
     <t>Viene segnalato un errore di token, ma il flusso applicativo prosegue con la produzione del referto. La correzione può essere fatta da un utente amministratore, tramite front-end</t>
   </si>
   <si>
-    <t>Viene segnalato un errore di timeout, ma il flusso applicativo prosegue con la produzione del referto. La correzione può essere fatta da un utente amministratore, tramite front-end</t>
-  </si>
-  <si>
     <t>Viene segnalato l'errore ritornato dal Gateway. La correzione può essere fatta da un utente amministratore, tramite front-end, attivando l'obbligatorietà del campo</t>
   </si>
   <si>
@@ -4798,6 +4795,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.180.4.4.437a9ef12b45b2793ed712f7c2cc1966b18754462e7d19c4a05f8fb699543c0a.172908bf2f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene segnalato l'errore di token, ma il flusso applicativo prosegue con la produzione del referto. La correzione può essere fatta da un utente amministratore, tramite front-end</t>
   </si>
 </sst>
 </file>
@@ -5216,6 +5216,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5237,9 +5240,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7703,10 +7703,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I156" sqref="I156"/>
+      <selection pane="bottomRight" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7748,14 +7748,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
         <v>913</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="37"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7773,14 +7773,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="45" t="s">
         <v>910</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="37"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7798,12 +7798,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="45" t="s">
         <v>911</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7822,12 +7822,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45" t="s">
         <v>912</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7845,8 +7845,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -9288,7 +9288,7 @@
         <v>845</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>941</v>
+        <v>956</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26" t="s">
@@ -12995,13 +12995,13 @@
         <v>45272</v>
       </c>
       <c r="G155" s="24" t="s">
-        <v>948</v>
-      </c>
-      <c r="H155" s="45" t="s">
-        <v>951</v>
-      </c>
-      <c r="I155" s="45" t="s">
-        <v>954</v>
+        <v>947</v>
+      </c>
+      <c r="H155" s="33" t="s">
+        <v>950</v>
+      </c>
+      <c r="I155" s="33" t="s">
+        <v>953</v>
       </c>
       <c r="J155" s="25" t="s">
         <v>136</v>
@@ -13041,13 +13041,13 @@
         <v>45272</v>
       </c>
       <c r="G156" s="24" t="s">
-        <v>949</v>
-      </c>
-      <c r="H156" s="45" t="s">
-        <v>952</v>
-      </c>
-      <c r="I156" s="45" t="s">
-        <v>955</v>
+        <v>948</v>
+      </c>
+      <c r="H156" s="33" t="s">
+        <v>951</v>
+      </c>
+      <c r="I156" s="33" t="s">
+        <v>954</v>
       </c>
       <c r="J156" s="25" t="s">
         <v>136</v>
@@ -13086,14 +13086,14 @@
       <c r="F157" s="23">
         <v>45272</v>
       </c>
-      <c r="G157" s="45" t="s">
-        <v>950</v>
-      </c>
-      <c r="H157" s="45" t="s">
-        <v>953</v>
-      </c>
-      <c r="I157" s="45" t="s">
-        <v>956</v>
+      <c r="G157" s="33" t="s">
+        <v>949</v>
+      </c>
+      <c r="H157" s="33" t="s">
+        <v>952</v>
+      </c>
+      <c r="I157" s="33" t="s">
+        <v>955</v>
       </c>
       <c r="J157" s="25" t="s">
         <v>136</v>
@@ -13158,7 +13158,7 @@
         <v>845</v>
       </c>
       <c r="P158" s="25" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="Q158" s="25"/>
       <c r="R158" s="26" t="s">
@@ -13214,7 +13214,7 @@
         <v>845</v>
       </c>
       <c r="P159" s="25" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="Q159" s="25"/>
       <c r="R159" s="26" t="s">
@@ -13270,7 +13270,7 @@
         <v>845</v>
       </c>
       <c r="P160" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q160" s="25"/>
       <c r="R160" s="26" t="s">
@@ -13326,7 +13326,7 @@
         <v>845</v>
       </c>
       <c r="P161" s="25" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Q161" s="25"/>
       <c r="R161" s="26" t="s">
@@ -13382,7 +13382,7 @@
         <v>845</v>
       </c>
       <c r="P162" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q162" s="25"/>
       <c r="R162" s="26" t="s">
@@ -13438,7 +13438,7 @@
         <v>845</v>
       </c>
       <c r="P163" s="25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26" t="s">
@@ -13494,7 +13494,7 @@
         <v>845</v>
       </c>
       <c r="P164" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q164" s="25"/>
       <c r="R164" s="26" t="s">
@@ -13550,7 +13550,7 @@
         <v>845</v>
       </c>
       <c r="P165" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q165" s="25"/>
       <c r="R165" s="26" t="s">
@@ -13606,7 +13606,7 @@
         <v>845</v>
       </c>
       <c r="P166" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q166" s="25"/>
       <c r="R166" s="26" t="s">
@@ -13662,7 +13662,7 @@
         <v>845</v>
       </c>
       <c r="P167" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26" t="s">
@@ -13718,7 +13718,7 @@
         <v>845</v>
       </c>
       <c r="P168" s="25" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26" t="s">
@@ -13774,7 +13774,7 @@
         <v>845</v>
       </c>
       <c r="P169" s="25" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Q169" s="25"/>
       <c r="R169" s="26" t="s">
@@ -13830,7 +13830,7 @@
         <v>845</v>
       </c>
       <c r="P170" s="25" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Q170" s="25"/>
       <c r="R170" s="26" t="s">
@@ -13886,7 +13886,7 @@
         <v>845</v>
       </c>
       <c r="P171" s="25" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Q171" s="25"/>
       <c r="R171" s="26" t="s">
@@ -13942,7 +13942,7 @@
         <v>845</v>
       </c>
       <c r="P172" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q172" s="25"/>
       <c r="R172" s="26" t="s">
@@ -13998,7 +13998,7 @@
         <v>845</v>
       </c>
       <c r="P173" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q173" s="25"/>
       <c r="R173" s="26" t="s">
@@ -14054,7 +14054,7 @@
         <v>845</v>
       </c>
       <c r="P174" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q174" s="25"/>
       <c r="R174" s="26" t="s">
@@ -14110,7 +14110,7 @@
         <v>845</v>
       </c>
       <c r="P175" s="25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Q175" s="25"/>
       <c r="R175" s="26" t="s">
@@ -14166,7 +14166,7 @@
         <v>845</v>
       </c>
       <c r="P176" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="Q176" s="25"/>
       <c r="R176" s="26" t="s">

</xml_diff>